<commit_message>
add license plate for card
</commit_message>
<xml_diff>
--- a/Parking Server/src/Zero.Web.Mvc/wwwroot/assets/SampleFiles/Import_TheXe.xlsx
+++ b/Parking Server/src/Zero.Web.Mvc/wwwroot/assets/SampleFiles/Import_TheXe.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Ghi chú</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>Tên loại xe</t>
+  </si>
+  <si>
+    <t>Số dư</t>
+  </si>
+  <si>
+    <t>Biển số</t>
   </si>
 </sst>
 </file>
@@ -669,22 +675,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:F14518"/>
+  <dimension ref="A1:H14518"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" customWidth="1"/>
+    <col min="6" max="6" width="32" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="115.15" customHeight="1">
+    <row r="1" spans="1:8" ht="115.15" customHeight="1">
       <c r="A1" s="20" t="s">
         <v>3</v>
       </c>
@@ -697,77 +705,89 @@
       <c r="D1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="15"/>
-    </row>
-    <row r="2" spans="1:6" ht="67.900000000000006" customHeight="1">
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:8" ht="67.900000000000006" customHeight="1">
       <c r="A2" s="21"/>
       <c r="B2" s="22"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="1:6" ht="42.4" customHeight="1">
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="1:8" ht="42.4" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="16"/>
       <c r="C3" s="17"/>
       <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
-    </row>
-    <row r="4" spans="1:6" ht="39.4" customHeight="1">
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
+    </row>
+    <row r="4" spans="1:8" ht="39.4" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="1:6" ht="49.9" customHeight="1">
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" ht="49.9" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:8">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75">
+    <row r="9" spans="1:8" ht="15.75">
       <c r="A9" s="1"/>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:8">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:8">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:8">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:8">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:8">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:8">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:8">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
     </row>
@@ -58780,12 +58800,14 @@
       <c r="B14518" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
+    <mergeCell ref="G1:G2"/>
     <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>